<commit_message>
reimported ASSAY as instances
</commit_message>
<xml_diff>
--- a/docs/ANLYMD_PRVAM.xlsx
+++ b/docs/ANLYMD_PRVAM.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fernanda.dorea\Documents\GitHub\HSO\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2FBFCA-CBAD-416A-9BC0-85A409082973}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A2C9F0-C13C-4AF5-90FB-95E876CDBF1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13707" activeTab="2" xr2:uid="{553E772C-41C9-4095-A335-145E91CB48EF}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="13707" activeTab="3" xr2:uid="{553E772C-41C9-4095-A335-145E91CB48EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="root" sheetId="2" r:id="rId2"/>
     <sheet name="subclasses" sheetId="3" r:id="rId3"/>
+    <sheet name="hierarchy lost" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Blad1!$A$1:$F$113</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="516">
   <si>
     <t>URI</t>
   </si>
@@ -1956,11 +1957,14 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection sqref="A1:F101"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4250,13 +4254,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE988C3B-4D0D-4974-A6B3-AFDF3DD54F72}">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B57"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.375" customWidth="1"/>
+    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.125" customWidth="1"/>
     <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
@@ -5411,8 +5415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55E3DF7E-B0D3-4A80-8F0B-C1BD2418C4BF}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B57"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -6571,4 +6575,2284 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6649B2DF-D1E0-4097-8206-43E8410DB7FC}">
+  <dimension ref="A1:F113"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.125" customWidth="1"/>
+    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>400</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>407</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>400</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>408</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>400</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>409</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>400</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>411</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" t="s">
+        <v>400</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>412</v>
+      </c>
+      <c r="B10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" t="s">
+        <v>400</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>413</v>
+      </c>
+      <c r="B11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" t="s">
+        <v>400</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>414</v>
+      </c>
+      <c r="B12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" t="s">
+        <v>400</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>415</v>
+      </c>
+      <c r="B13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C13" t="s">
+        <v>400</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>416</v>
+      </c>
+      <c r="B14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C14" t="s">
+        <v>400</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>417</v>
+      </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15" t="s">
+        <v>400</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>418</v>
+      </c>
+      <c r="B16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" t="s">
+        <v>400</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>419</v>
+      </c>
+      <c r="B17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" t="s">
+        <v>400</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" t="s">
+        <v>176</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>420</v>
+      </c>
+      <c r="B18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C18" t="s">
+        <v>400</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>421</v>
+      </c>
+      <c r="B19" t="s">
+        <v>180</v>
+      </c>
+      <c r="C19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E19" t="s">
+        <v>181</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>422</v>
+      </c>
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" t="s">
+        <v>400</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>423</v>
+      </c>
+      <c r="B21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C21" t="s">
+        <v>400</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>424</v>
+      </c>
+      <c r="B22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" t="s">
+        <v>400</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>425</v>
+      </c>
+      <c r="B23" t="s">
+        <v>189</v>
+      </c>
+      <c r="C23" t="s">
+        <v>400</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>426</v>
+      </c>
+      <c r="B24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C24" t="s">
+        <v>400</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>427</v>
+      </c>
+      <c r="B25" t="s">
+        <v>193</v>
+      </c>
+      <c r="C25" t="s">
+        <v>400</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>428</v>
+      </c>
+      <c r="B26" t="s">
+        <v>198</v>
+      </c>
+      <c r="C26" t="s">
+        <v>400</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>429</v>
+      </c>
+      <c r="B27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" t="s">
+        <v>400</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>430</v>
+      </c>
+      <c r="B28" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" t="s">
+        <v>400</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>431</v>
+      </c>
+      <c r="B29" t="s">
+        <v>208</v>
+      </c>
+      <c r="C29" t="s">
+        <v>400</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>432</v>
+      </c>
+      <c r="B30" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" t="s">
+        <v>400</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>433</v>
+      </c>
+      <c r="B31" t="s">
+        <v>212</v>
+      </c>
+      <c r="C31" t="s">
+        <v>400</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>434</v>
+      </c>
+      <c r="B32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C32" t="s">
+        <v>400</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E32" t="s">
+        <v>215</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>435</v>
+      </c>
+      <c r="B33" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" t="s">
+        <v>400</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>436</v>
+      </c>
+      <c r="B34" t="s">
+        <v>219</v>
+      </c>
+      <c r="C34" t="s">
+        <v>400</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>437</v>
+      </c>
+      <c r="B35" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" t="s">
+        <v>400</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>438</v>
+      </c>
+      <c r="B36" t="s">
+        <v>223</v>
+      </c>
+      <c r="C36" t="s">
+        <v>400</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>439</v>
+      </c>
+      <c r="B37" t="s">
+        <v>225</v>
+      </c>
+      <c r="C37" t="s">
+        <v>400</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>440</v>
+      </c>
+      <c r="B38" t="s">
+        <v>227</v>
+      </c>
+      <c r="C38" t="s">
+        <v>400</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>441</v>
+      </c>
+      <c r="B39" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" t="s">
+        <v>400</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>442</v>
+      </c>
+      <c r="B40" t="s">
+        <v>236</v>
+      </c>
+      <c r="C40" t="s">
+        <v>400</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E40" t="s">
+        <v>237</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>443</v>
+      </c>
+      <c r="B41" t="s">
+        <v>239</v>
+      </c>
+      <c r="C41" t="s">
+        <v>400</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>444</v>
+      </c>
+      <c r="B42" t="s">
+        <v>246</v>
+      </c>
+      <c r="C42" t="s">
+        <v>400</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>445</v>
+      </c>
+      <c r="B43" t="s">
+        <v>248</v>
+      </c>
+      <c r="C43" t="s">
+        <v>400</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E43" t="s">
+        <v>249</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>446</v>
+      </c>
+      <c r="B44" t="s">
+        <v>251</v>
+      </c>
+      <c r="C44" t="s">
+        <v>400</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E44" t="s">
+        <v>252</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>447</v>
+      </c>
+      <c r="B45" t="s">
+        <v>254</v>
+      </c>
+      <c r="C45" t="s">
+        <v>400</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E45" t="s">
+        <v>255</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>448</v>
+      </c>
+      <c r="B46" t="s">
+        <v>261</v>
+      </c>
+      <c r="C46" t="s">
+        <v>400</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>449</v>
+      </c>
+      <c r="B47" t="s">
+        <v>263</v>
+      </c>
+      <c r="C47" t="s">
+        <v>400</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>450</v>
+      </c>
+      <c r="B48" t="s">
+        <v>265</v>
+      </c>
+      <c r="C48" t="s">
+        <v>400</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E48" t="s">
+        <v>166</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>451</v>
+      </c>
+      <c r="B49" t="s">
+        <v>267</v>
+      </c>
+      <c r="C49" t="s">
+        <v>400</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E49" t="s">
+        <v>268</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>452</v>
+      </c>
+      <c r="B50" t="s">
+        <v>270</v>
+      </c>
+      <c r="C50" t="s">
+        <v>400</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>453</v>
+      </c>
+      <c r="B51" t="s">
+        <v>272</v>
+      </c>
+      <c r="C51" t="s">
+        <v>400</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>454</v>
+      </c>
+      <c r="B52" t="s">
+        <v>274</v>
+      </c>
+      <c r="C52" t="s">
+        <v>400</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E52" t="s">
+        <v>275</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>455</v>
+      </c>
+      <c r="B53" t="s">
+        <v>277</v>
+      </c>
+      <c r="C53" t="s">
+        <v>400</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>456</v>
+      </c>
+      <c r="B54" t="s">
+        <v>279</v>
+      </c>
+      <c r="C54" t="s">
+        <v>400</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>457</v>
+      </c>
+      <c r="B55" t="s">
+        <v>281</v>
+      </c>
+      <c r="C55" t="s">
+        <v>400</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>458</v>
+      </c>
+      <c r="B56" t="s">
+        <v>283</v>
+      </c>
+      <c r="C56" t="s">
+        <v>400</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E56" t="s">
+        <v>284</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>459</v>
+      </c>
+      <c r="B57" t="s">
+        <v>286</v>
+      </c>
+      <c r="C57" t="s">
+        <v>400</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E57" t="s">
+        <v>287</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>460</v>
+      </c>
+      <c r="B58" t="s">
+        <v>14</v>
+      </c>
+      <c r="C58" t="s">
+        <v>400</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>461</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>400</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" t="s">
+        <v>15</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>462</v>
+      </c>
+      <c r="B60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C60" t="s">
+        <v>400</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>463</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" t="s">
+        <v>400</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" t="s">
+        <v>15</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>464</v>
+      </c>
+      <c r="B62" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" t="s">
+        <v>400</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E62" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>465</v>
+      </c>
+      <c r="B63" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" t="s">
+        <v>400</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63" t="s">
+        <v>15</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>466</v>
+      </c>
+      <c r="B64" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" t="s">
+        <v>400</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" t="s">
+        <v>15</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>467</v>
+      </c>
+      <c r="B65" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" t="s">
+        <v>400</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>468</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>400</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E66" t="s">
+        <v>43</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>469</v>
+      </c>
+      <c r="B67" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" t="s">
+        <v>400</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E67" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>470</v>
+      </c>
+      <c r="B68" t="s">
+        <v>48</v>
+      </c>
+      <c r="C68" t="s">
+        <v>400</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E68" t="s">
+        <v>49</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>471</v>
+      </c>
+      <c r="B69" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69" t="s">
+        <v>400</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E69" t="s">
+        <v>52</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>472</v>
+      </c>
+      <c r="B70" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" t="s">
+        <v>400</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E70" t="s">
+        <v>55</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>473</v>
+      </c>
+      <c r="B71" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71" t="s">
+        <v>400</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E71" t="s">
+        <v>58</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>474</v>
+      </c>
+      <c r="B72" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" t="s">
+        <v>400</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E72" t="s">
+        <v>61</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>475</v>
+      </c>
+      <c r="B73" t="s">
+        <v>63</v>
+      </c>
+      <c r="C73" t="s">
+        <v>400</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E73" t="s">
+        <v>64</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>476</v>
+      </c>
+      <c r="B74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C74" t="s">
+        <v>400</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E74" t="s">
+        <v>67</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>477</v>
+      </c>
+      <c r="B75" t="s">
+        <v>69</v>
+      </c>
+      <c r="C75" t="s">
+        <v>400</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E75" t="s">
+        <v>70</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>478</v>
+      </c>
+      <c r="B76" t="s">
+        <v>72</v>
+      </c>
+      <c r="C76" t="s">
+        <v>400</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E76" t="s">
+        <v>73</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>479</v>
+      </c>
+      <c r="B77" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E77" t="s">
+        <v>15</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>480</v>
+      </c>
+      <c r="B78" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" t="s">
+        <v>400</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E78" t="s">
+        <v>78</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>481</v>
+      </c>
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C79" t="s">
+        <v>400</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E79" t="s">
+        <v>81</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>482</v>
+      </c>
+      <c r="B80" t="s">
+        <v>83</v>
+      </c>
+      <c r="C80" t="s">
+        <v>400</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E80" t="s">
+        <v>84</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>483</v>
+      </c>
+      <c r="B81" t="s">
+        <v>86</v>
+      </c>
+      <c r="C81" t="s">
+        <v>400</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E81" t="s">
+        <v>87</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>484</v>
+      </c>
+      <c r="B82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82" t="s">
+        <v>400</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E82" t="s">
+        <v>90</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>485</v>
+      </c>
+      <c r="B83" t="s">
+        <v>92</v>
+      </c>
+      <c r="C83" t="s">
+        <v>400</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E83" t="s">
+        <v>90</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>486</v>
+      </c>
+      <c r="B84" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84" t="s">
+        <v>400</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E84" t="s">
+        <v>95</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>487</v>
+      </c>
+      <c r="B85" t="s">
+        <v>97</v>
+      </c>
+      <c r="C85" t="s">
+        <v>400</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E85" t="s">
+        <v>98</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>488</v>
+      </c>
+      <c r="B86" t="s">
+        <v>100</v>
+      </c>
+      <c r="C86" t="s">
+        <v>400</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E86" t="s">
+        <v>101</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>489</v>
+      </c>
+      <c r="B87" t="s">
+        <v>103</v>
+      </c>
+      <c r="C87" t="s">
+        <v>400</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E87" t="s">
+        <v>104</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>490</v>
+      </c>
+      <c r="B88" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" t="s">
+        <v>400</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E88" t="s">
+        <v>15</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>491</v>
+      </c>
+      <c r="B89" t="s">
+        <v>108</v>
+      </c>
+      <c r="C89" t="s">
+        <v>400</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E89" t="s">
+        <v>15</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>492</v>
+      </c>
+      <c r="B90" t="s">
+        <v>110</v>
+      </c>
+      <c r="C90" t="s">
+        <v>400</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E90" t="s">
+        <v>111</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>493</v>
+      </c>
+      <c r="B91" t="s">
+        <v>113</v>
+      </c>
+      <c r="C91" t="s">
+        <v>400</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E91" t="s">
+        <v>114</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>494</v>
+      </c>
+      <c r="B92" t="s">
+        <v>116</v>
+      </c>
+      <c r="C92" t="s">
+        <v>400</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E92" t="s">
+        <v>117</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>495</v>
+      </c>
+      <c r="B93" t="s">
+        <v>119</v>
+      </c>
+      <c r="C93" t="s">
+        <v>400</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E93" t="s">
+        <v>120</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>496</v>
+      </c>
+      <c r="B94" t="s">
+        <v>122</v>
+      </c>
+      <c r="C94" t="s">
+        <v>400</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E94" t="s">
+        <v>123</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>497</v>
+      </c>
+      <c r="B95" t="s">
+        <v>125</v>
+      </c>
+      <c r="C95" t="s">
+        <v>400</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E95" t="s">
+        <v>126</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>498</v>
+      </c>
+      <c r="B96" t="s">
+        <v>128</v>
+      </c>
+      <c r="C96" t="s">
+        <v>400</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E96" t="s">
+        <v>129</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>499</v>
+      </c>
+      <c r="B97" t="s">
+        <v>131</v>
+      </c>
+      <c r="C97" t="s">
+        <v>400</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E97" t="s">
+        <v>132</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>500</v>
+      </c>
+      <c r="B98" t="s">
+        <v>134</v>
+      </c>
+      <c r="C98" t="s">
+        <v>400</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E98" t="s">
+        <v>135</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>501</v>
+      </c>
+      <c r="B99" t="s">
+        <v>137</v>
+      </c>
+      <c r="C99" t="s">
+        <v>400</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E99" t="s">
+        <v>138</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>502</v>
+      </c>
+      <c r="B100" t="s">
+        <v>140</v>
+      </c>
+      <c r="C100" t="s">
+        <v>400</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E100" t="s">
+        <v>141</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>503</v>
+      </c>
+      <c r="B101" t="s">
+        <v>143</v>
+      </c>
+      <c r="C101" t="s">
+        <v>400</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E101" t="s">
+        <v>144</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>504</v>
+      </c>
+      <c r="B102" t="s">
+        <v>146</v>
+      </c>
+      <c r="C102" t="s">
+        <v>400</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E102" t="s">
+        <v>147</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>505</v>
+      </c>
+      <c r="B103" t="s">
+        <v>154</v>
+      </c>
+      <c r="C103" t="s">
+        <v>400</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E103" t="s">
+        <v>15</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>506</v>
+      </c>
+      <c r="B104" t="s">
+        <v>168</v>
+      </c>
+      <c r="C104" t="s">
+        <v>400</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E104" t="s">
+        <v>169</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>507</v>
+      </c>
+      <c r="B105" t="s">
+        <v>195</v>
+      </c>
+      <c r="C105" t="s">
+        <v>400</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E105" t="s">
+        <v>196</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>508</v>
+      </c>
+      <c r="B106" t="s">
+        <v>200</v>
+      </c>
+      <c r="C106" t="s">
+        <v>400</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E106" t="s">
+        <v>15</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>509</v>
+      </c>
+      <c r="B107" t="s">
+        <v>202</v>
+      </c>
+      <c r="C107" t="s">
+        <v>400</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E107" t="s">
+        <v>15</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>510</v>
+      </c>
+      <c r="B108" t="s">
+        <v>229</v>
+      </c>
+      <c r="C108" t="s">
+        <v>400</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E108" t="s">
+        <v>15</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>511</v>
+      </c>
+      <c r="B109" t="s">
+        <v>233</v>
+      </c>
+      <c r="C109" t="s">
+        <v>400</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E109" t="s">
+        <v>234</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>512</v>
+      </c>
+      <c r="B110" t="s">
+        <v>241</v>
+      </c>
+      <c r="C110" t="s">
+        <v>400</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E110" t="s">
+        <v>242</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>513</v>
+      </c>
+      <c r="B111" t="s">
+        <v>244</v>
+      </c>
+      <c r="C111" t="s">
+        <v>400</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E111" t="s">
+        <v>15</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>514</v>
+      </c>
+      <c r="B112" t="s">
+        <v>257</v>
+      </c>
+      <c r="C112" t="s">
+        <v>400</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E112" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>515</v>
+      </c>
+      <c r="B113" t="s">
+        <v>259</v>
+      </c>
+      <c r="C113" t="s">
+        <v>400</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E113" t="s">
+        <v>15</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>